<commit_message>
spacecraft.py is the main file, which uses spaceFormulae as the calculations module. Thus spacecraft.py interfaces the excel sheet to the calculations module and for now outputs the downlink SNR for each s/c.
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TUDelftSID\Documents\GitHub\ADSEE-2-Group-Assignment-for-Spacecraft-and-Aircraft\Spacecraft\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Other\python\projects\AE2111\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023A0E98-1B66-41C0-B568-48362284F949}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FAC230-7686-4823-B291-9C65E576E6FB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14076" yWindow="2136" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>Earth #U CubeSat</t>
-  </si>
-  <si>
     <t>Moon 12U Cubesat</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>Required BER</t>
+  </si>
+  <si>
+    <t>Earth 3U CubeSat</t>
   </si>
 </sst>
 </file>
@@ -562,13 +562,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="27.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -576,27 +579,27 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="27.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="4">
         <v>10</v>
@@ -614,12 +617,12 @@
         <v>800</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="40.1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4">
         <v>2</v>
@@ -637,12 +640,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="53" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="4">
         <v>400</v>
@@ -660,12 +663,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="40.1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="5">
         <v>0.8</v>
@@ -683,12 +686,12 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3">
         <v>0.7</v>
@@ -706,12 +709,12 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="26.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C7" s="3">
         <v>2.2000000000000002</v>
@@ -729,12 +732,12 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="39.4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <f>221/240</f>
@@ -757,12 +760,12 @@
         <v>0.85113636363636369</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="26.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C9">
         <v>0.1</v>
@@ -780,12 +783,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="39.4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -803,12 +806,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="26.5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="C11">
         <v>350</v>
@@ -826,18 +829,18 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="26.5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E12">
         <v>10</v>
@@ -849,12 +852,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="39.4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -872,12 +875,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="39.4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C14">
         <f>10^7</f>
@@ -900,12 +903,12 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="59.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -923,12 +926,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="26.5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16">
         <v>0.1</v>
@@ -946,12 +949,12 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="39.4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17">
         <v>8</v>
@@ -969,12 +972,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="26.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C18" s="7">
         <v>1</v>
@@ -992,12 +995,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="39.4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="C19">
         <v>0.5</v>
@@ -1015,35 +1018,35 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="39.4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>8</v>
+      </c>
+      <c r="G20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="26.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C20">
-        <v>8</v>
-      </c>
-      <c r="D20">
-        <v>8</v>
-      </c>
-      <c r="E20">
-        <v>8</v>
-      </c>
-      <c r="F20">
-        <v>8</v>
-      </c>
-      <c r="G20">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="27" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="B21" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21">
         <f>10^-6</f>

</xml_diff>

<commit_message>
Added the BIRD example spacecraft link budget data to the excel sheet for cross-checking the calculations
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Other\python\projects\AE2111\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FAC230-7686-4823-B291-9C65E576E6FB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B2890F-F337-47F1-AB87-8A06E9A4080B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>Parameter</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Earth 3U CubeSat</t>
+  </si>
+  <si>
+    <t>BIRD (example question from last lecture)</t>
   </si>
 </sst>
 </file>
@@ -227,25 +230,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,45 +563,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="3" max="8" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" ht="14.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="27.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" ht="14.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="4">
@@ -616,12 +627,19 @@
       <c r="G2" s="4">
         <v>800</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="40.1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="H2" s="9">
+        <v>40</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" ht="14.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="4">
@@ -639,12 +657,19 @@
       <c r="G3" s="4">
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="53" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="H3" s="9">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" ht="14.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4">
@@ -662,12 +687,19 @@
       <c r="G4" s="4">
         <v>1000</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="40.1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="H4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" ht="14.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="5">
@@ -685,389 +717,620 @@
       <c r="G5" s="5">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="H5" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="6">
         <v>0.7</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="6">
         <v>0.7</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>0.7</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="6">
         <v>0.7</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="6">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="26.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="H6" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="6">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="6">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="6">
         <v>8.4</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="6">
         <v>8.5</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="6">
         <v>8.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="39.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="H7" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <f>221/240</f>
         <v>0.92083333333333328</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <f>221/240</f>
         <v>0.92083333333333328</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <f>749/880</f>
         <v>0.85113636363636369</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <f t="shared" ref="F8:G8" si="0">749/880</f>
         <v>0.85113636363636369</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>0.85113636363636369</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="26.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="H8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>0.1</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>0.3</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <v>1</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>1.5</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="39.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="H9" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>5</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>10</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>34</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="26.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="H10" s="12">
+        <v>10</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>350</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>1000</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <v>500</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>800</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>500</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="26.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="H11" s="12">
+        <v>570</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <v>10</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>20</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="39.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="H12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>5</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>1</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <v>1</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>0.05</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="39.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="H13" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <f>10^7</f>
         <v>10000000</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <f>10^6</f>
         <v>1000000</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3">
         <f>10^5</f>
         <v>100000</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="3">
         <f>10^4</f>
         <v>10000</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="3">
         <f>10^3</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="59.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="H14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>20</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>30</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="3">
         <v>30</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="3">
         <v>45</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="3">
         <v>45</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="26.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="H15" s="3">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>0.1</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>0.1</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="3">
         <v>0.2</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <v>0.05</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="3">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="39.4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="H16" s="3">
+        <v>21600</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="3">
         <v>8</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <v>8</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="3">
         <v>8</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <v>8</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="26.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="H17" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="8">
         <v>1</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="8">
         <v>0.5</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="8">
         <v>1</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="8">
         <v>0.5</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="39.4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="H18" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="3">
         <v>0.5</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <v>6</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="3">
         <v>12</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3">
         <v>24</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="39.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="H19" s="3">
+        <v>2</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <v>8</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <v>8</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="3">
         <v>8</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>8</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="26.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="H20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <f>10^-6</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <f t="shared" ref="D21:G21" si="1">10^-6</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="3">
         <f t="shared" si="1"/>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <f t="shared" si="1"/>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="3">
         <f t="shared" si="1"/>
         <v>9.9999999999999995E-7</v>
       </c>
+      <c r="H21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Marked all cells that we cannot change in the linkdata file. Also put the data for the ADCS questions in the adcsdata file
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Other\python\projects\AE2111\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B2890F-F337-47F1-AB87-8A06E9A4080B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8BEEB6-45CE-49D7-A0A5-8D57086B4BB7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -175,52 +175,23 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFAFAF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -230,31 +201,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFAFAF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -563,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -575,762 +557,776 @@
     <col min="3" max="8" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" ht="14.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="6">
         <v>10</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="6">
         <v>40</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="6">
         <v>20</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="6">
         <v>1200</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="6">
         <v>800</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="7">
         <v>40</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" ht="14.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="8">
         <v>2</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="8">
         <v>8</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="8">
         <v>5</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="8">
         <v>350</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="8">
         <v>150</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="7">
         <v>2</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" ht="14.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="8">
         <v>400</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="8">
         <v>400</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="8">
         <v>400</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="8">
         <v>1000</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="8">
         <v>1000</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" ht="14.3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="9">
         <v>0.8</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="9">
         <v>0.8</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="9">
         <v>0.8</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="9">
         <v>0.9</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="9">
         <v>0.9</v>
       </c>
       <c r="H5" s="10">
         <v>0.8</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
     </row>
     <row r="6" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="11">
         <v>0.7</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="11">
         <v>0.7</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="11">
         <v>0.7</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="11">
         <v>0.7</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="11">
         <v>0.7</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="1">
         <v>0.8</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="12">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="11">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="12">
         <v>8.4</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="12">
         <v>8.5</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="12">
         <v>8.4</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="1">
         <v>2.5</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="13">
         <f>221/240</f>
         <v>0.92083333333333328</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="5">
         <f>221/240</f>
         <v>0.92083333333333328</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="13">
         <f>749/880</f>
         <v>0.85113636363636369</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="13">
         <f t="shared" ref="F8:G8" si="0">749/880</f>
         <v>0.85113636363636369</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>0.85113636363636369</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="5">
         <v>0.1</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="13">
         <v>0.3</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="13">
         <v>1</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="13">
         <v>1.5</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="5">
         <v>3</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="2">
         <v>0.5</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="13">
         <v>1</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="13">
         <v>5</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="5">
         <v>10</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="5">
         <v>34</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="13">
         <v>70</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="2">
         <v>10</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
     </row>
     <row r="11" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="5">
         <v>350</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="13">
         <v>1000</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="5">
         <v>500</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="13">
         <v>800</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="13">
         <v>500</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="2">
         <v>570</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="13">
         <v>10</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="13">
         <v>20</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="13">
         <v>10</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="5">
         <v>5</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="5">
         <v>1</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="5">
         <v>1</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="5">
         <v>0.05</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="5">
         <v>0.05</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="2">
         <v>0.25</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
     </row>
     <row r="14" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="13">
         <f>10^7</f>
         <v>10000000</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="13">
         <f>10^6</f>
         <v>1000000</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="13">
         <f>10^5</f>
         <v>100000</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="13">
         <f>10^4</f>
         <v>10000</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="13">
         <f>10^3</f>
         <v>1000</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="5">
         <v>20</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="13">
         <v>30</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="13">
         <v>30</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="5">
         <v>45</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="5">
         <v>45</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="5">
         <v>1</v>
       </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
     </row>
     <row r="16" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="13">
         <v>0.1</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="13">
         <v>0.1</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="5">
         <v>0.2</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="13">
         <v>0.05</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="5">
         <v>0.01</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="5">
         <v>21600</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="13">
         <v>8</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="13">
         <v>8</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="13">
         <v>8</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="13">
         <v>8</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="13">
         <v>8</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="14">
         <v>1000000</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="15">
         <v>1</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="15">
         <v>0.5</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="16">
         <v>1</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="15">
         <v>0.5</v>
       </c>
-      <c r="G18" s="8">
-        <v>1</v>
-      </c>
-      <c r="H18" s="8">
+      <c r="G18" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="H18" s="15">
         <v>0.5</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="13">
         <v>0.5</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="5">
         <v>6</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="5">
         <v>12</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="5">
         <v>24</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="13">
         <v>24</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="5">
         <v>2</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
     </row>
     <row r="20" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="5">
         <v>8</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="5">
         <v>8</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="5">
         <v>8</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="5">
         <v>8</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="5">
         <v>8</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="13">
         <f>10^-6</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="13">
         <f t="shared" ref="D21:G21" si="1">10^-6</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="13">
         <f t="shared" si="1"/>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="13">
         <f t="shared" si="1"/>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="13">
         <f t="shared" si="1"/>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Added SNR margin calculations, interplanetary distance calculations
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Other\python\projects\AE2111\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8BEEB6-45CE-49D7-A0A5-8D57086B4BB7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AF72FE-6B56-49A9-A149-D9DB02D3329D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15704" yWindow="4904" windowWidth="19562" windowHeight="10257" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Parameter</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>BIRD (example question from last lecture)</t>
+  </si>
+  <si>
+    <t>S/C-Sun distance</t>
   </si>
 </sst>
 </file>
@@ -201,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -226,6 +229,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -924,28 +928,28 @@
     </row>
     <row r="13" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="5">
-        <v>5</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1</v>
-      </c>
-      <c r="E13" s="5">
-        <v>1</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0.25</v>
+        <v>20</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="18">
+        <v>227900000</v>
+      </c>
+      <c r="F13" s="18">
+        <v>108200000</v>
+      </c>
+      <c r="G13" s="18">
+        <v>780000000</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -954,33 +958,28 @@
     </row>
     <row r="14" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="13">
-        <f>10^7</f>
-        <v>10000000</v>
-      </c>
-      <c r="D14" s="13">
-        <f>10^6</f>
-        <v>1000000</v>
-      </c>
-      <c r="E14" s="13">
-        <f>10^5</f>
-        <v>100000</v>
-      </c>
-      <c r="F14" s="13">
-        <f>10^4</f>
-        <v>10000</v>
-      </c>
-      <c r="G14" s="13">
-        <f>10^3</f>
-        <v>1000</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="C14" s="5">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.25</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -989,28 +988,33 @@
     </row>
     <row r="15" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="5">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="C15" s="13">
+        <f>10^7</f>
+        <v>10000000</v>
       </c>
       <c r="D15" s="13">
-        <v>30</v>
+        <f>10^6</f>
+        <v>1000000</v>
       </c>
       <c r="E15" s="13">
-        <v>30</v>
-      </c>
-      <c r="F15" s="5">
-        <v>45</v>
-      </c>
-      <c r="G15" s="5">
-        <v>45</v>
-      </c>
-      <c r="H15" s="5">
-        <v>1</v>
+        <f>10^5</f>
+        <v>100000</v>
+      </c>
+      <c r="F15" s="13">
+        <f>10^4</f>
+        <v>10000</v>
+      </c>
+      <c r="G15" s="13">
+        <f>10^3</f>
+        <v>1000</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1019,28 +1023,28 @@
     </row>
     <row r="16" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="5">
+        <v>20</v>
+      </c>
+      <c r="D16" s="13">
         <v>30</v>
       </c>
-      <c r="C16" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="D16" s="13">
-        <v>0.1</v>
-      </c>
-      <c r="E16" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="F16" s="13">
-        <v>0.05</v>
+      <c r="E16" s="13">
+        <v>30</v>
+      </c>
+      <c r="F16" s="5">
+        <v>45</v>
       </c>
       <c r="G16" s="5">
-        <v>0.01</v>
+        <v>45</v>
       </c>
       <c r="H16" s="5">
-        <v>21600</v>
+        <v>1</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -1049,28 +1053,28 @@
     </row>
     <row r="17" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>11</v>
+        <v>28</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="C17" s="13">
-        <v>8</v>
+        <v>0.1</v>
       </c>
       <c r="D17" s="13">
-        <v>8</v>
-      </c>
-      <c r="E17" s="13">
-        <v>8</v>
+        <v>0.1</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.2</v>
       </c>
       <c r="F17" s="13">
-        <v>8</v>
-      </c>
-      <c r="G17" s="13">
-        <v>8</v>
-      </c>
-      <c r="H17" s="14">
-        <v>1000000</v>
+        <v>0.05</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="H17" s="5">
+        <v>21600</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -1079,28 +1083,28 @@
     </row>
     <row r="18" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="15">
-        <v>1</v>
-      </c>
-      <c r="D18" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="E18" s="16">
-        <v>1</v>
-      </c>
-      <c r="F18" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="G18" s="16">
-        <v>0.75</v>
-      </c>
-      <c r="H18" s="15">
-        <v>0.5</v>
+      <c r="C18" s="13">
+        <v>8</v>
+      </c>
+      <c r="D18" s="13">
+        <v>8</v>
+      </c>
+      <c r="E18" s="13">
+        <v>8</v>
+      </c>
+      <c r="F18" s="13">
+        <v>8</v>
+      </c>
+      <c r="G18" s="13">
+        <v>8</v>
+      </c>
+      <c r="H18" s="14">
+        <v>1000000</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -1109,28 +1113,28 @@
     </row>
     <row r="19" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="13">
+        <v>11</v>
+      </c>
+      <c r="C19" s="15">
+        <v>1</v>
+      </c>
+      <c r="D19" s="15">
         <v>0.5</v>
       </c>
-      <c r="D19" s="5">
-        <v>6</v>
-      </c>
-      <c r="E19" s="5">
-        <v>12</v>
-      </c>
-      <c r="F19" s="5">
-        <v>24</v>
-      </c>
-      <c r="G19" s="13">
-        <v>24</v>
-      </c>
-      <c r="H19" s="5">
-        <v>2</v>
+      <c r="E19" s="16">
+        <v>1</v>
+      </c>
+      <c r="F19" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="G19" s="16">
+        <v>0.75</v>
+      </c>
+      <c r="H19" s="15">
+        <v>0.5</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -1139,28 +1143,28 @@
     </row>
     <row r="20" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="5">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="C20" s="13">
+        <v>0.5</v>
       </c>
       <c r="D20" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E20" s="5">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F20" s="5">
-        <v>8</v>
-      </c>
-      <c r="G20" s="5">
-        <v>8</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="G20" s="13">
+        <v>24</v>
+      </c>
+      <c r="H20" s="5">
+        <v>2</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -1169,30 +1173,25 @@
     </row>
     <row r="21" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="13">
-        <f>10^-6</f>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D21" s="13">
-        <f t="shared" ref="D21:G21" si="1">10^-6</f>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="E21" s="13">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="F21" s="13">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="G21" s="13">
-        <f t="shared" si="1"/>
-        <v>9.9999999999999995E-7</v>
+        <v>35</v>
+      </c>
+      <c r="C21" s="5">
+        <v>8</v>
+      </c>
+      <c r="D21" s="5">
+        <v>8</v>
+      </c>
+      <c r="E21" s="5">
+        <v>8</v>
+      </c>
+      <c r="F21" s="5">
+        <v>8</v>
+      </c>
+      <c r="G21" s="5">
+        <v>8</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>23</v>
@@ -1202,15 +1201,36 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+    <row r="22" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="13">
+        <f>10^-6</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D22" s="13">
+        <f t="shared" ref="D22:G22" si="1">10^-6</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="E22" s="13">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F22" s="13">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="G22" s="13">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -1315,18 +1335,32 @@
       <c r="L29" s="5"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Added required SNR calculations and made an original copy of the linkdata.xlsx so we can alter the current version to close the link budget and still compare it to the original
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Other\python\projects\AE2111\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AF72FE-6B56-49A9-A149-D9DB02D3329D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C671FED7-5A27-425C-A99D-21BE9DF3711B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15704" yWindow="4904" windowWidth="19562" windowHeight="10257" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="503" yWindow="503" windowWidth="19562" windowHeight="10256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>Parameter</t>
   </si>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -877,7 +877,7 @@
         <v>350</v>
       </c>
       <c r="D11" s="13">
-        <v>1000</v>
+        <v>384400</v>
       </c>
       <c r="E11" s="5">
         <v>500</v>
@@ -1193,8 +1193,8 @@
       <c r="G21" s="5">
         <v>8</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>23</v>
+      <c r="H21" s="5">
+        <v>8</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -1228,8 +1228,9 @@
         <f t="shared" si="1"/>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="H22" s="5" t="s">
-        <v>23</v>
+      <c r="H22" s="5">
+        <f>0.000001</f>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>

</xml_diff>

<commit_message>
Added a transmitter power for the BIRD S/C to the linkdata
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Other\python\projects\AE2111\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C671FED7-5A27-425C-A99D-21BE9DF3711B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072E4B74-E1B6-4F32-9657-3BDEF5EA52F9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="503" yWindow="503" windowWidth="19562" windowHeight="10256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2663" yWindow="2663" windowWidth="19562" windowHeight="10256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>Parameter</t>
   </si>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -613,7 +613,7 @@
       <c r="G2" s="6">
         <v>800</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="8">
         <v>40</v>
       </c>
       <c r="I2" s="5"/>
@@ -673,8 +673,8 @@
       <c r="G4" s="8">
         <v>1000</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>23</v>
+      <c r="H4" s="11">
+        <v>400</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>

</xml_diff>

<commit_message>
Edits to Europa mission
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Other\python\projects\AE2111\Spacecraft\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grey Phoenix\Documents\GitHub\ADSEE-2-Group-Assignment-for-Spacecraft-and-Aircraft\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072E4B74-E1B6-4F32-9657-3BDEF5EA52F9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273656DA-4551-4F5A-84CA-AC3D6DCB2B0C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2663" yWindow="2663" windowWidth="19562" windowHeight="10256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14125" yWindow="3940" windowWidth="7763" windowHeight="9426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,51 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={41A8A4C3-DE19-4F63-B6D8-7BF6D8A86538}</author>
+    <author>tc={5176026F-5461-4E32-A34B-4414CAA79E07}</author>
+    <author>tc={0187DFA3-534F-42FC-9602-F80762B81959}</author>
+    <author>tc={7560B4A9-64D3-447A-9174-00395EDA3828}</author>
+  </authors>
+  <commentList>
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{41A8A4C3-DE19-4F63-B6D8-7BF6D8A86538}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Increase power 150 -&gt; 400</t>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="1" shapeId="0" xr:uid="{5176026F-5461-4E32-A34B-4414CAA79E07}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Voyager's was 3.7m</t>
+      </text>
+    </comment>
+    <comment ref="G16" authorId="2" shapeId="0" xr:uid="{0187DFA3-534F-42FC-9602-F80762B81959}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    OG: 45</t>
+      </text>
+    </comment>
+    <comment ref="G17" authorId="3" shapeId="0" xr:uid="{7560B4A9-64D3-447A-9174-00395EDA3828}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    0.05</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
@@ -157,7 +202,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +221,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -204,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -230,6 +288,7 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -250,6 +309,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Andries Nusselder" id="{5E9D8826-9B1A-435C-95AF-0D5D65C354EF}" userId="492cd1201a6c86c6" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -547,21 +612,39 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G3" dT="2019-10-11T20:44:25.37" personId="{5E9D8826-9B1A-435C-95AF-0D5D65C354EF}" id="{41A8A4C3-DE19-4F63-B6D8-7BF6D8A86538}">
+    <text>Increase power 150 -&gt; 400</text>
+  </threadedComment>
+  <threadedComment ref="G9" dT="2019-10-11T20:22:54.92" personId="{5E9D8826-9B1A-435C-95AF-0D5D65C354EF}" id="{5176026F-5461-4E32-A34B-4414CAA79E07}">
+    <text>Voyager's was 3.7m</text>
+  </threadedComment>
+  <threadedComment ref="G16" dT="2019-10-11T20:45:03.25" personId="{5E9D8826-9B1A-435C-95AF-0D5D65C354EF}" id="{0187DFA3-534F-42FC-9602-F80762B81959}">
+    <text>OG: 45</text>
+  </threadedComment>
+  <threadedComment ref="G17" dT="2019-10-11T20:45:22.36" personId="{5E9D8826-9B1A-435C-95AF-0D5D65C354EF}" id="{7560B4A9-64D3-447A-9174-00395EDA3828}">
+    <text>0.05</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="3" max="8" width="18.625" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -591,11 +674,11 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="6">
@@ -621,7 +704,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -641,7 +724,7 @@
         <v>350</v>
       </c>
       <c r="G3" s="8">
-        <v>150</v>
+        <v>400</v>
       </c>
       <c r="H3" s="7">
         <v>2</v>
@@ -651,7 +734,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -681,7 +764,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -711,7 +794,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -741,7 +824,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -771,7 +854,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -806,7 +889,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -826,7 +909,7 @@
         <v>1.5</v>
       </c>
       <c r="G9" s="5">
-        <v>3</v>
+        <v>3.7</v>
       </c>
       <c r="H9" s="2">
         <v>0.5</v>
@@ -836,7 +919,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -866,7 +949,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -896,7 +979,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
@@ -926,7 +1009,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>39</v>
       </c>
@@ -956,7 +1039,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
@@ -986,7 +1069,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -1021,7 +1104,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -1041,7 +1124,7 @@
         <v>45</v>
       </c>
       <c r="G16" s="5">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="H16" s="5">
         <v>1</v>
@@ -1051,7 +1134,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
@@ -1071,7 +1154,7 @@
         <v>0.05</v>
       </c>
       <c r="G17" s="5">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="H17" s="5">
         <v>21600</v>
@@ -1081,7 +1164,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
@@ -1111,7 +1194,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>31</v>
       </c>
@@ -1141,7 +1224,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
@@ -1171,7 +1254,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
@@ -1201,7 +1284,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>36</v>
       </c>
@@ -1237,7 +1320,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1251,7 +1334,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1265,7 +1348,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1279,7 +1362,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1293,7 +1376,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1307,7 +1390,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1321,7 +1404,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1335,7 +1418,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1349,7 +1432,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
@@ -1367,5 +1450,6 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added pdf assignment files, finished the Venus Explorer link budget
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grey Phoenix\Documents\GitHub\ADSEE-2-Group-Assignment-for-Spacecraft-and-Aircraft\Spacecraft\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TUDelftSID\Documents\GitHub\ADSEE-2-Group-Assignment-for-Spacecraft-and-Aircraft\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273656DA-4551-4F5A-84CA-AC3D6DCB2B0C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181BD354-9C0A-4C3C-AF38-1F61E38C1FCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14125" yWindow="3940" windowWidth="7763" windowHeight="9426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11160" yWindow="1344" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,10 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={41A8A4C3-DE19-4F63-B6D8-7BF6D8A86538}</author>
+    <author>tc={C0F54C17-50C2-461C-BA4D-33A277D4CB25}</author>
     <author>tc={5176026F-5461-4E32-A34B-4414CAA79E07}</author>
+    <author>tc={57BB61D0-CF2D-442A-A42A-ECAE6ED2383A}</author>
+    <author>tc={D0AAE9CA-DDBB-4208-AE53-81519D4399F1}</author>
     <author>tc={0187DFA3-534F-42FC-9602-F80762B81959}</author>
     <author>tc={7560B4A9-64D3-447A-9174-00395EDA3828}</author>
   </authors>
@@ -47,7 +50,17 @@
     Increase power 150 -&gt; 400</t>
       </text>
     </comment>
-    <comment ref="G9" authorId="1" shapeId="0" xr:uid="{5176026F-5461-4E32-A34B-4414CAA79E07}">
+    <comment ref="F6" authorId="1" shapeId="0" xr:uid="{C0F54C17-50C2-461C-BA4D-33A277D4CB25}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    OG: 0.7
+Reply:
+    BIRD: 0.8</t>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="2" shapeId="0" xr:uid="{5176026F-5461-4E32-A34B-4414CAA79E07}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -55,7 +68,35 @@
     Voyager's was 3.7m</t>
       </text>
     </comment>
-    <comment ref="G16" authorId="2" shapeId="0" xr:uid="{0187DFA3-534F-42FC-9602-F80762B81959}">
+    <comment ref="F10" authorId="3" shapeId="0" xr:uid="{57BB61D0-CF2D-442A-A42A-ECAE6ED2383A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    OG:34
+Reply:
+    https://deepspace.jpl.nasa.gov/about/complexes/70-meter/
+Reply:
+    https://en.wikipedia.org/wiki/Madrid_Deep_Space_Communications_Complex
+Reply:
+    https://en.wikipedia.org/wiki/Canberra_Deep_Space_Communication_Complex
+Reply:
+    https://en.wikipedia.org/wiki/Yevpatoria_RT-70_radio_telescope
+Reply:
+    https://en.wikipedia.org/wiki/Galenki_RT-70_radio_telescope</t>
+      </text>
+    </comment>
+    <comment ref="F16" authorId="4" shapeId="0" xr:uid="{D0AAE9CA-DDBB-4208-AE53-81519D4399F1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    OG:45
+Reply:
+    BIRD: 1</t>
+      </text>
+    </comment>
+    <comment ref="G16" authorId="5" shapeId="0" xr:uid="{0187DFA3-534F-42FC-9602-F80762B81959}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -63,7 +104,7 @@
     OG: 45</t>
       </text>
     </comment>
-    <comment ref="G17" authorId="3" shapeId="0" xr:uid="{7560B4A9-64D3-447A-9174-00395EDA3828}">
+    <comment ref="G17" authorId="6" shapeId="0" xr:uid="{7560B4A9-64D3-447A-9174-00395EDA3828}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -233,7 +274,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -314,6 +355,7 @@
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Andries Nusselder" id="{5E9D8826-9B1A-435C-95AF-0D5D65C354EF}" userId="492cd1201a6c86c6" providerId="Windows Live"/>
+  <person displayName="Varvara Isidorova" id="{0E41E7B7-3EA0-4ADB-874B-1A59CAA944AE}" userId="Varvara Isidorova" providerId="None"/>
 </personList>
 </file>
 
@@ -617,8 +659,38 @@
   <threadedComment ref="G3" dT="2019-10-11T20:44:25.37" personId="{5E9D8826-9B1A-435C-95AF-0D5D65C354EF}" id="{41A8A4C3-DE19-4F63-B6D8-7BF6D8A86538}">
     <text>Increase power 150 -&gt; 400</text>
   </threadedComment>
+  <threadedComment ref="F6" dT="2019-10-13T11:06:35.91" personId="{0E41E7B7-3EA0-4ADB-874B-1A59CAA944AE}" id="{C0F54C17-50C2-461C-BA4D-33A277D4CB25}">
+    <text>OG: 0.7</text>
+  </threadedComment>
+  <threadedComment ref="F6" dT="2019-10-13T12:52:36.11" personId="{0E41E7B7-3EA0-4ADB-874B-1A59CAA944AE}" id="{942910A2-37B6-42F6-AC1F-9BF24E1AB1BB}" parentId="{C0F54C17-50C2-461C-BA4D-33A277D4CB25}">
+    <text>BIRD: 0.8</text>
+  </threadedComment>
   <threadedComment ref="G9" dT="2019-10-11T20:22:54.92" personId="{5E9D8826-9B1A-435C-95AF-0D5D65C354EF}" id="{5176026F-5461-4E32-A34B-4414CAA79E07}">
     <text>Voyager's was 3.7m</text>
+  </threadedComment>
+  <threadedComment ref="F10" dT="2019-10-13T11:07:24.98" personId="{0E41E7B7-3EA0-4ADB-874B-1A59CAA944AE}" id="{57BB61D0-CF2D-442A-A42A-ECAE6ED2383A}">
+    <text>OG:34</text>
+  </threadedComment>
+  <threadedComment ref="F10" dT="2019-10-13T11:20:10.45" personId="{0E41E7B7-3EA0-4ADB-874B-1A59CAA944AE}" id="{0501680C-79F6-4E32-8D54-42DEFFE0051B}" parentId="{57BB61D0-CF2D-442A-A42A-ECAE6ED2383A}">
+    <text>https://deepspace.jpl.nasa.gov/about/complexes/70-meter/</text>
+  </threadedComment>
+  <threadedComment ref="F10" dT="2019-10-13T11:22:12.53" personId="{0E41E7B7-3EA0-4ADB-874B-1A59CAA944AE}" id="{AA5D5813-554C-4476-BF76-0ED5979C82A5}" parentId="{57BB61D0-CF2D-442A-A42A-ECAE6ED2383A}">
+    <text>https://en.wikipedia.org/wiki/Madrid_Deep_Space_Communications_Complex</text>
+  </threadedComment>
+  <threadedComment ref="F10" dT="2019-10-13T11:22:29.90" personId="{0E41E7B7-3EA0-4ADB-874B-1A59CAA944AE}" id="{22009B6E-1FD0-4523-B6A4-1A6F55B5479B}" parentId="{57BB61D0-CF2D-442A-A42A-ECAE6ED2383A}">
+    <text>https://en.wikipedia.org/wiki/Canberra_Deep_Space_Communication_Complex</text>
+  </threadedComment>
+  <threadedComment ref="F10" dT="2019-10-13T11:23:21.89" personId="{0E41E7B7-3EA0-4ADB-874B-1A59CAA944AE}" id="{4FF932C5-3462-44EC-8C2F-DF292CEB056D}" parentId="{57BB61D0-CF2D-442A-A42A-ECAE6ED2383A}">
+    <text>https://en.wikipedia.org/wiki/Yevpatoria_RT-70_radio_telescope</text>
+  </threadedComment>
+  <threadedComment ref="F10" dT="2019-10-13T11:24:09.81" personId="{0E41E7B7-3EA0-4ADB-874B-1A59CAA944AE}" id="{2F60F2CD-F230-4286-B497-9C61D74052E2}" parentId="{57BB61D0-CF2D-442A-A42A-ECAE6ED2383A}">
+    <text>https://en.wikipedia.org/wiki/Galenki_RT-70_radio_telescope</text>
+  </threadedComment>
+  <threadedComment ref="F16" dT="2019-10-13T11:10:17.54" personId="{0E41E7B7-3EA0-4ADB-874B-1A59CAA944AE}" id="{D0AAE9CA-DDBB-4208-AE53-81519D4399F1}">
+    <text>OG:45</text>
+  </threadedComment>
+  <threadedComment ref="F16" dT="2019-10-13T12:52:52.07" personId="{0E41E7B7-3EA0-4ADB-874B-1A59CAA944AE}" id="{8572F600-B1E0-4AF6-BD18-4983BA06AFEB}" parentId="{D0AAE9CA-DDBB-4208-AE53-81519D4399F1}">
+    <text>BIRD: 1</text>
   </threadedComment>
   <threadedComment ref="G16" dT="2019-10-11T20:45:03.25" personId="{5E9D8826-9B1A-435C-95AF-0D5D65C354EF}" id="{0187DFA3-534F-42FC-9602-F80762B81959}">
     <text>OG: 45</text>
@@ -635,10 +707,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G4" sqref="G4"/>
+      <selection pane="topRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="8" width="18.6640625" customWidth="1"/>
@@ -811,7 +883,7 @@
         <v>0.7</v>
       </c>
       <c r="F6" s="11">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="G6" s="11">
         <v>0.7</v>
@@ -936,7 +1008,7 @@
         <v>10</v>
       </c>
       <c r="F10" s="5">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="G10" s="13">
         <v>70</v>
@@ -1121,7 +1193,7 @@
         <v>30</v>
       </c>
       <c r="F16" s="5">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="G16" s="5">
         <v>1</v>

</xml_diff>

<commit_message>
Changing values of Europa
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grey Phoenix\Documents\GitHub\ADSEE-2-Group-Assignment-for-Spacecraft-and-Aircraft\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273656DA-4551-4F5A-84CA-AC3D6DCB2B0C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13596647-B5C9-4BC4-8E01-9F9669C698BB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14125" yWindow="3940" windowWidth="7763" windowHeight="9426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -289,6 +289,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,14 +639,18 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G4" sqref="G4"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="18.6640625" customWidth="1"/>
+    <col min="3" max="6" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -663,7 +672,7 @@
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -877,7 +886,7 @@
         <f t="shared" ref="F8:G8" si="0">749/880</f>
         <v>0.85113636363636369</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="12">
         <f t="shared" si="0"/>
         <v>0.85113636363636369</v>
       </c>
@@ -908,7 +917,7 @@
       <c r="F9" s="13">
         <v>1.5</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="11">
         <v>3.7</v>
       </c>
       <c r="H9" s="2">
@@ -938,7 +947,7 @@
       <c r="F10" s="5">
         <v>34</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="12">
         <v>70</v>
       </c>
       <c r="H10" s="2">
@@ -968,7 +977,7 @@
       <c r="F11" s="13">
         <v>800</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="12">
         <v>500</v>
       </c>
       <c r="H11" s="2">
@@ -998,7 +1007,7 @@
       <c r="F12" s="13">
         <v>20</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="12">
         <v>10</v>
       </c>
       <c r="H12" s="5" t="s">
@@ -1028,7 +1037,7 @@
       <c r="F13" s="18">
         <v>108200000</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="12">
         <v>780000000</v>
       </c>
       <c r="H13" s="5" t="s">
@@ -1058,7 +1067,7 @@
       <c r="F14" s="5">
         <v>0.05</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="11">
         <v>0.05</v>
       </c>
       <c r="H14" s="2">
@@ -1092,7 +1101,7 @@
         <f>10^4</f>
         <v>10000</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="12">
         <f>10^3</f>
         <v>1000</v>
       </c>
@@ -1123,8 +1132,8 @@
       <c r="F16" s="5">
         <v>45</v>
       </c>
-      <c r="G16" s="5">
-        <v>1</v>
+      <c r="G16" s="22">
+        <v>0.28444439999999999</v>
       </c>
       <c r="H16" s="5">
         <v>1</v>
@@ -1153,8 +1162,9 @@
       <c r="F17" s="13">
         <v>0.05</v>
       </c>
-      <c r="G17" s="5">
-        <v>1</v>
+      <c r="G17" s="11">
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
       </c>
       <c r="H17" s="5">
         <v>21600</v>
@@ -1183,7 +1193,7 @@
       <c r="F18" s="13">
         <v>8</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="12">
         <v>8</v>
       </c>
       <c r="H18" s="14">
@@ -1213,7 +1223,7 @@
       <c r="F19" s="15">
         <v>0.5</v>
       </c>
-      <c r="G19" s="16">
+      <c r="G19" s="12">
         <v>0.75</v>
       </c>
       <c r="H19" s="15">
@@ -1243,7 +1253,7 @@
       <c r="F20" s="5">
         <v>24</v>
       </c>
-      <c r="G20" s="13">
+      <c r="G20" s="12">
         <v>24</v>
       </c>
       <c r="H20" s="5">
@@ -1273,7 +1283,7 @@
       <c r="F21" s="5">
         <v>8</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="11">
         <v>8</v>
       </c>
       <c r="H21" s="5">
@@ -1284,41 +1294,41 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:12" s="23" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="18">
         <f>10^-6</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="18">
         <f t="shared" ref="D22:G22" si="1">10^-6</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="18">
         <f t="shared" si="1"/>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="18">
         <f t="shared" si="1"/>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="18">
         <f t="shared" si="1"/>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="22">
         <f>0.000001</f>
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
@@ -1327,7 +1337,7 @@
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="G23" s="11"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -1341,7 +1351,7 @@
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="G24" s="11"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
@@ -1355,7 +1365,7 @@
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="G25" s="11"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
@@ -1369,7 +1379,7 @@
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="G26" s="11"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
@@ -1383,7 +1393,7 @@
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+      <c r="G27" s="11"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
@@ -1397,7 +1407,7 @@
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+      <c r="G28" s="11"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
@@ -1411,7 +1421,7 @@
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="G29" s="11"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
@@ -1425,7 +1435,7 @@
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+      <c r="G30" s="11"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
@@ -1439,7 +1449,7 @@
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
       <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
+      <c r="G31" s="20"/>
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
       <c r="J31" s="17"/>

</xml_diff>

<commit_message>
Added flag to spacecraft.py so you can calculate the original link budget from original_linkdata.xlsx
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TUDelftSID\Documents\GitHub\ADSEE-2-Group-Assignment-for-Spacecraft-and-Aircraft\Spacecraft\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Other\python\projects\AE2111\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181BD354-9C0A-4C3C-AF38-1F61E38C1FCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C354E0-065B-4544-8E24-21A64B77D705}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="1344" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,7 @@
     <author>tc={57BB61D0-CF2D-442A-A42A-ECAE6ED2383A}</author>
     <author>tc={D0AAE9CA-DDBB-4208-AE53-81519D4399F1}</author>
     <author>tc={0187DFA3-534F-42FC-9602-F80762B81959}</author>
+    <author>tc={7399D209-54FE-48F2-8880-EC0ED569771C}</author>
     <author>tc={7560B4A9-64D3-447A-9174-00395EDA3828}</author>
   </authors>
   <commentList>
@@ -93,7 +94,9 @@
 Comment:
     OG:45
 Reply:
-    BIRD: 1</t>
+    BIRD: 1
+Reply:
+    BIRD payload data is mock data to generate 1e6 bit/s, so the actual dimensions are bullshit, they only amount to 1e6 in total</t>
       </text>
     </comment>
     <comment ref="G16" authorId="5" shapeId="0" xr:uid="{0187DFA3-534F-42FC-9602-F80762B81959}">
@@ -104,7 +107,17 @@
     OG: 45</t>
       </text>
     </comment>
-    <comment ref="G17" authorId="6" shapeId="0" xr:uid="{7560B4A9-64D3-447A-9174-00395EDA3828}">
+    <comment ref="H16" authorId="6" shapeId="0" xr:uid="{7399D209-54FE-48F2-8880-EC0ED569771C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This data is bullshit
+Reply:
+    It was made to give a data rate of 1e6 bit/s</t>
+      </text>
+    </comment>
+    <comment ref="G17" authorId="7" shapeId="0" xr:uid="{7560B4A9-64D3-447A-9174-00395EDA3828}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -354,6 +367,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Paul Eckstein" id="{105B921C-CE61-41BE-8CA1-0AD662A83714}" userId="Paul Eckstein" providerId="None"/>
   <person displayName="Andries Nusselder" id="{5E9D8826-9B1A-435C-95AF-0D5D65C354EF}" userId="492cd1201a6c86c6" providerId="Windows Live"/>
   <person displayName="Varvara Isidorova" id="{0E41E7B7-3EA0-4ADB-874B-1A59CAA944AE}" userId="Varvara Isidorova" providerId="None"/>
 </personList>
@@ -692,8 +706,17 @@
   <threadedComment ref="F16" dT="2019-10-13T12:52:52.07" personId="{0E41E7B7-3EA0-4ADB-874B-1A59CAA944AE}" id="{8572F600-B1E0-4AF6-BD18-4983BA06AFEB}" parentId="{D0AAE9CA-DDBB-4208-AE53-81519D4399F1}">
     <text>BIRD: 1</text>
   </threadedComment>
+  <threadedComment ref="F16" dT="2019-10-14T12:41:27.67" personId="{105B921C-CE61-41BE-8CA1-0AD662A83714}" id="{94B1B9A0-B0FB-4187-B904-F831800D3001}" parentId="{D0AAE9CA-DDBB-4208-AE53-81519D4399F1}">
+    <text>BIRD payload data is mock data to generate 1e6 bit/s, so the actual dimensions are bullshit, they only amount to 1e6 in total</text>
+  </threadedComment>
   <threadedComment ref="G16" dT="2019-10-11T20:45:03.25" personId="{5E9D8826-9B1A-435C-95AF-0D5D65C354EF}" id="{0187DFA3-534F-42FC-9602-F80762B81959}">
     <text>OG: 45</text>
+  </threadedComment>
+  <threadedComment ref="H16" dT="2019-10-14T12:41:54.20" personId="{105B921C-CE61-41BE-8CA1-0AD662A83714}" id="{7399D209-54FE-48F2-8880-EC0ED569771C}">
+    <text>This data is bullshit</text>
+  </threadedComment>
+  <threadedComment ref="H16" dT="2019-10-14T12:42:19.88" personId="{105B921C-CE61-41BE-8CA1-0AD662A83714}" id="{A08FD0E4-AEF7-4207-B0AE-A866525B7B1F}" parentId="{7399D209-54FE-48F2-8880-EC0ED569771C}">
+    <text>It was made to give a data rate of 1e6 bit/s</text>
   </threadedComment>
   <threadedComment ref="G17" dT="2019-10-11T20:45:22.36" personId="{5E9D8826-9B1A-435C-95AF-0D5D65C354EF}" id="{7560B4A9-64D3-447A-9174-00395EDA3828}">
     <text>0.05</text>
@@ -706,17 +729,18 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F24" sqref="F24"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="H16"/>
+      <selection pane="topRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="18.6640625" customWidth="1"/>
+    <col min="3" max="8" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -746,7 +770,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -776,7 +800,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -790,7 +814,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="8">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F3" s="8">
         <v>350</v>
@@ -806,7 +830,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -820,7 +844,7 @@
         <v>400</v>
       </c>
       <c r="E4" s="8">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="F4" s="8">
         <v>1000</v>
@@ -836,7 +860,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -866,7 +890,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -880,7 +904,7 @@
         <v>0.7</v>
       </c>
       <c r="E6" s="11">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="F6" s="11">
         <v>0.8</v>
@@ -896,7 +920,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -926,7 +950,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -961,7 +985,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -991,7 +1015,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -1005,7 +1029,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="5">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="F10" s="5">
         <v>70</v>
@@ -1021,7 +1045,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -1051,7 +1075,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
@@ -1081,7 +1105,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>39</v>
       </c>
@@ -1111,7 +1135,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
@@ -1141,7 +1165,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -1176,7 +1200,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -1206,7 +1230,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
@@ -1220,7 +1244,7 @@
         <v>0.1</v>
       </c>
       <c r="E17" s="5">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F17" s="13">
         <v>0.05</v>
@@ -1236,7 +1260,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
@@ -1266,7 +1290,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>31</v>
       </c>
@@ -1296,7 +1320,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
@@ -1310,7 +1334,7 @@
         <v>6</v>
       </c>
       <c r="E20" s="5">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F20" s="5">
         <v>24</v>
@@ -1326,7 +1350,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
@@ -1356,7 +1380,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>36</v>
       </c>
@@ -1392,7 +1416,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1406,7 +1430,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1420,7 +1444,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1434,7 +1458,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1448,7 +1472,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1462,7 +1486,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1476,7 +1500,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1490,7 +1514,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1504,7 +1528,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>

</xml_diff>

<commit_message>
Added payload generated data calculations (dependent on orbit size etc..). Still debugging the code for a reason why the data rate is so high, until then please don't use!!
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grey Phoenix\Documents\GitHub\ADSEE-2-Group-Assignment-for-Spacecraft-and-Aircraft\Spacecraft\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Other\python\projects\AE2111\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13596647-B5C9-4BC4-8E01-9F9669C698BB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D35DF25-2920-4AE8-BB92-4CAAEFC35328}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14125" yWindow="3940" windowWidth="7763" windowHeight="9426" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>Parameter</t>
   </si>
@@ -196,13 +196,31 @@
   </si>
   <si>
     <t>S/C-Sun distance</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>Moon</t>
+  </si>
+  <si>
+    <t>Mars</t>
+  </si>
+  <si>
+    <t>Parent body</t>
+  </si>
+  <si>
+    <t>Venus</t>
+  </si>
+  <si>
+    <t>Europa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,12 +245,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -639,21 +651,21 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="21" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="3" max="6" width="18.625" customWidth="1"/>
+    <col min="7" max="7" width="18.625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -683,7 +695,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -713,7 +725,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -743,7 +755,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -773,7 +785,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -803,7 +815,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -833,7 +845,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -863,7 +875,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -898,7 +910,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -928,7 +940,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -958,7 +970,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -969,7 +981,7 @@
         <v>350</v>
       </c>
       <c r="D11" s="13">
-        <v>384400</v>
+        <v>1000</v>
       </c>
       <c r="E11" s="5">
         <v>500</v>
@@ -988,7 +1000,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
@@ -1018,7 +1030,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>39</v>
       </c>
@@ -1048,7 +1060,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
@@ -1078,7 +1090,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -1113,7 +1125,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -1143,7 +1155,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
@@ -1174,7 +1186,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
@@ -1204,7 +1216,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>31</v>
       </c>
@@ -1234,7 +1246,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
@@ -1264,7 +1276,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
@@ -1294,7 +1306,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" s="23" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" s="23" customFormat="1" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
         <v>36</v>
       </c>
@@ -1330,21 +1342,37 @@
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="5"/>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1358,7 +1386,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1372,7 +1400,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1386,7 +1414,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1400,7 +1428,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1414,7 +1442,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1428,29 +1456,21 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="5"/>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="17"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="17"/>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I31" s="17"/>
       <c r="J31" s="17"/>
       <c r="K31" s="17"/>

</xml_diff>

<commit_message>
Data rate bug seems fixed: conversion from arcminutes to degrees is now using the correct factor of 60
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Other\python\projects\AE2111\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D35DF25-2920-4AE8-BB92-4CAAEFC35328}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D868BC-D2A5-4FD1-BEB7-AED1D3CE9070}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3777" windowWidth="19562" windowHeight="10256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -654,7 +654,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1179,7 @@
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="H17" s="5">
-        <v>21600</v>
+        <v>60</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>

</xml_diff>

<commit_message>
work in progress, this is an intermediate version, working on the Earth 3U cubesat
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Other\python\projects\AE2111\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D868BC-D2A5-4FD1-BEB7-AED1D3CE9070}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60ADA3D9-1DB4-4360-B0E8-55956EEE3EA4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3777" windowWidth="19562" windowHeight="10256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8654" yWindow="2459" windowWidth="19563" windowHeight="10256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -654,7 +654,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -733,7 +733,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D3" s="8">
         <v>8</v>
@@ -918,7 +918,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="5">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="D9" s="13">
         <v>0.3</v>
@@ -978,7 +978,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="5">
-        <v>350</v>
+        <v>700</v>
       </c>
       <c r="D11" s="13">
         <v>1000</v>

</xml_diff>

<commit_message>
Earth 3U cubesat link budget is done!
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Other\python\projects\AE2111\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0EF46E-2028-4996-8AE9-E38387BC2609}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DAA1D3-E0E2-47A7-A9F8-F01460257845}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9333" yWindow="4891" windowWidth="19562" windowHeight="10256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
   <si>
     <t>Parameter</t>
   </si>
@@ -657,7 +657,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -766,7 +766,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="8">
-        <v>400</v>
+        <v>10</v>
       </c>
       <c r="D4" s="8">
         <v>400</v>
@@ -1227,7 +1227,7 @@
         <v>11</v>
       </c>
       <c r="C19" s="15">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="D19" s="15">
         <v>0.5</v>
@@ -1301,8 +1301,8 @@
       <c r="G21" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H21" s="5">
-        <v>8</v>
+      <c r="H21" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>

</xml_diff>

<commit_message>
All link budget up to and including Mars are done
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Other\python\projects\AE2111\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DAA1D3-E0E2-47A7-A9F8-F01460257845}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87547B8E-40BF-4340-841A-E4143D029BE4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9333" yWindow="4891" windowWidth="19562" windowHeight="10256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -657,7 +657,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -739,10 +739,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="8">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E3" s="8">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F3" s="8">
         <v>350</v>
@@ -769,10 +769,10 @@
         <v>10</v>
       </c>
       <c r="D4" s="8">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="E4" s="8">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="F4" s="8">
         <v>1000</v>
@@ -859,7 +859,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D7" s="11">
-        <v>2.2000000000000002</v>
+        <v>8.4</v>
       </c>
       <c r="E7" s="12">
         <v>8.4</v>
@@ -957,7 +957,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F10" s="5">
         <v>34</v>
@@ -987,7 +987,7 @@
         <v>1000</v>
       </c>
       <c r="E11" s="5">
-        <v>500</v>
+        <v>8000</v>
       </c>
       <c r="F11" s="13">
         <v>800</v>
@@ -1074,10 +1074,10 @@
         <v>2</v>
       </c>
       <c r="D14" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E14" s="5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F14" s="5">
         <v>0.05</v>
@@ -1172,7 +1172,7 @@
         <v>0.1</v>
       </c>
       <c r="E17" s="5">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="13">
         <v>0.05</v>
@@ -1230,7 +1230,7 @@
         <v>0.4</v>
       </c>
       <c r="D19" s="15">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="E19" s="16">
         <v>1</v>
@@ -1260,7 +1260,7 @@
         <v>0.5</v>
       </c>
       <c r="D20" s="5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E20" s="5">
         <v>12</v>
@@ -1290,10 +1290,10 @@
         <v>46</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
finished Venus as well
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Other\python\projects\AE2111\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87547B8E-40BF-4340-841A-E4143D029BE4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4776F09-C3E2-4275-8955-85FA4C7B52BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9333" yWindow="4891" windowWidth="19562" windowHeight="10256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -657,7 +657,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -745,7 +745,7 @@
         <v>15</v>
       </c>
       <c r="F3" s="8">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="G3" s="8">
         <v>400</v>
@@ -775,7 +775,7 @@
         <v>600</v>
       </c>
       <c r="F4" s="8">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="G4" s="8">
         <v>1000</v>
@@ -835,7 +835,7 @@
         <v>0.7</v>
       </c>
       <c r="F6" s="11">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="G6" s="11">
         <v>0.7</v>
@@ -960,7 +960,7 @@
         <v>50</v>
       </c>
       <c r="F10" s="5">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="G10" s="12">
         <v>70</v>
@@ -1145,7 +1145,7 @@
         <v>30</v>
       </c>
       <c r="F16" s="5">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="G16" s="22">
         <v>0.28444439999999999</v>
@@ -1236,7 +1236,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="15">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="G19" s="12">
         <v>0.75</v>
@@ -1296,7 +1296,7 @@
         <v>46</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Closed the Europa budget and changed the notation of the coding in the original as well to keep it compatible
</commit_message>
<xml_diff>
--- a/Spacecraft/linkdata.xlsx
+++ b/Spacecraft/linkdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grey Phoenix\Documents\GitHub\ADSEE-2-Group-Assignment-for-Spacecraft-and-Aircraft\Spacecraft\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Other\python\projects\AE2111\Spacecraft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3FEF91-D041-4562-825B-A0719DD85B44}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD901CF-F836-4B5B-91EA-FD7F86798E58}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4713" windowWidth="7763" windowHeight="9425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1902" yWindow="1902" windowWidth="22143" windowHeight="14142" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,6 @@
   <authors>
     <author>tc={41A8A4C3-DE19-4F63-B6D8-7BF6D8A86538}</author>
     <author>tc={5176026F-5461-4E32-A34B-4414CAA79E07}</author>
-    <author>tc={0187DFA3-534F-42FC-9602-F80762B81959}</author>
     <author>tc={7560B4A9-64D3-447A-9174-00395EDA3828}</author>
   </authors>
   <commentList>
@@ -55,15 +54,7 @@
     Voyager's was 3.7m</t>
       </text>
     </comment>
-    <comment ref="G16" authorId="2" shapeId="0" xr:uid="{0187DFA3-534F-42FC-9602-F80762B81959}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    OG: 45</t>
-      </text>
-    </comment>
-    <comment ref="G17" authorId="3" shapeId="0" xr:uid="{7560B4A9-64D3-447A-9174-00395EDA3828}">
+    <comment ref="G17" authorId="2" shapeId="0" xr:uid="{7560B4A9-64D3-447A-9174-00395EDA3828}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -640,9 +631,6 @@
   <threadedComment ref="G9" dT="2019-10-11T20:22:54.92" personId="{5E9D8826-9B1A-435C-95AF-0D5D65C354EF}" id="{5176026F-5461-4E32-A34B-4414CAA79E07}">
     <text>Voyager's was 3.7m</text>
   </threadedComment>
-  <threadedComment ref="G16" dT="2019-10-11T20:45:03.25" personId="{5E9D8826-9B1A-435C-95AF-0D5D65C354EF}" id="{0187DFA3-534F-42FC-9602-F80762B81959}">
-    <text>OG: 45</text>
-  </threadedComment>
   <threadedComment ref="G17" dT="2019-10-11T20:45:22.36" personId="{5E9D8826-9B1A-435C-95AF-0D5D65C354EF}" id="{7560B4A9-64D3-447A-9174-00395EDA3828}">
     <text>0.05</text>
   </threadedComment>
@@ -654,21 +642,21 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="21" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
+    <col min="3" max="6" width="18.625" customWidth="1"/>
+    <col min="7" max="7" width="18.625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -698,7 +686,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -728,7 +716,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -758,7 +746,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -778,7 +766,7 @@
         <v>100</v>
       </c>
       <c r="G4" s="8">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="H4" s="11">
         <v>400</v>
@@ -788,7 +776,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -818,7 +806,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -848,7 +836,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -878,7 +866,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -913,7 +901,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -943,7 +931,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -973,7 +961,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -1003,7 +991,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>21</v>
       </c>
@@ -1033,7 +1021,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>38</v>
       </c>
@@ -1063,7 +1051,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
@@ -1093,7 +1081,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -1128,7 +1116,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -1147,8 +1135,8 @@
       <c r="F16" s="5">
         <v>10</v>
       </c>
-      <c r="G16" s="22">
-        <v>2.4</v>
+      <c r="G16" s="5">
+        <v>0.4</v>
       </c>
       <c r="H16" s="5">
         <v>1</v>
@@ -1158,7 +1146,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
@@ -1189,7 +1177,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
@@ -1219,7 +1207,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>31</v>
       </c>
@@ -1249,7 +1237,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
@@ -1279,7 +1267,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>34</v>
       </c>
@@ -1309,7 +1297,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" s="23" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" s="23" customFormat="1" ht="14.3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
         <v>35</v>
       </c>
@@ -1345,7 +1333,7 @@
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>42</v>
       </c>
@@ -1375,7 +1363,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1389,7 +1377,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1403,7 +1391,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1417,7 +1405,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1431,7 +1419,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1445,7 +1433,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1459,7 +1447,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
@@ -1473,7 +1461,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="I31" s="17"/>
       <c r="J31" s="17"/>
       <c r="K31" s="17"/>

</xml_diff>